<commit_message>
modification of one incorrect random value Benoît
</commit_message>
<xml_diff>
--- a/data/cg_peakValueTime_vm.xlsx
+++ b/data/cg_peakValueTime_vm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benoît\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\travail\sourcecode\developing\paper\centriG\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90EC113-B63C-4F0C-8BB5-38FF19BB2B83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D6A050-CCA7-494E-8FB2-319837AF227F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1350" windowWidth="19560" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,7 +1340,7 @@
         <v>9.3379999999999992</v>
       </c>
       <c r="F14">
-        <v>13.323</v>
+        <v>10.323</v>
       </c>
       <c r="G14">
         <v>8.9510000000000005</v>

</xml_diff>